<commit_message>
3v3 reverse polarity FET, connected current monitor to ADC, defined RF PWM and ADC pins on 104 connector, added UART connector, pc104 reverse polarity FET, 104 connector TVS diode.
</commit_message>
<xml_diff>
--- a/demoboard_v2/0714spreadsheet.xlsx
+++ b/demoboard_v2/0714spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richard/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richard/SFUSat/obc-hardware/demoboard_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="170">
   <si>
     <t>TMS570LS0714</t>
   </si>
@@ -531,6 +531,18 @@
   </si>
   <si>
     <t>RF_CLK</t>
+  </si>
+  <si>
+    <t>RF_ADC1</t>
+  </si>
+  <si>
+    <t>RF_ADC2</t>
+  </si>
+  <si>
+    <t>RF_PWM1</t>
+  </si>
+  <si>
+    <t>RF_PWM2</t>
   </si>
 </sst>
 </file>
@@ -876,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="F143" sqref="F143"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,6 +1040,9 @@
       <c r="E10" t="s">
         <v>148</v>
       </c>
+      <c r="F10" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1045,6 +1060,9 @@
       <c r="E11" t="s">
         <v>148</v>
       </c>
+      <c r="F11" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1521,6 +1539,9 @@
       <c r="E39" t="s">
         <v>149</v>
       </c>
+      <c r="F39" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
@@ -1537,6 +1558,9 @@
       </c>
       <c r="E40" t="s">
         <v>149</v>
+      </c>
+      <c r="F40" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added debug LED and 1v2 good LED
</commit_message>
<xml_diff>
--- a/demoboard_v2/0714spreadsheet.xlsx
+++ b/demoboard_v2/0714spreadsheet.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="171">
   <si>
     <t>TMS570LS0714</t>
   </si>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t>RF_PWM2</t>
+  </si>
+  <si>
+    <t>Debug LED</t>
   </si>
 </sst>
 </file>
@@ -888,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1734,6 +1737,9 @@
       </c>
       <c r="E50" t="s">
         <v>71</v>
+      </c>
+      <c r="F50" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added clock, RTC, flash serial connections
</commit_message>
<xml_diff>
--- a/demoboard_v2/0714spreadsheet.xlsx
+++ b/demoboard_v2/0714spreadsheet.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="172">
   <si>
     <t>TMS570LS0714</t>
   </si>
@@ -546,6 +546,9 @@
   </si>
   <si>
     <t>Debug LED</t>
+  </si>
+  <si>
+    <t>GIOB2 test point</t>
   </si>
 </sst>
 </file>
@@ -891,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,6 +1028,9 @@
       </c>
       <c r="E9" t="s">
         <v>148</v>
+      </c>
+      <c r="F9" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished watchdog circuit. Todo: add footprint for tact switch, i2c, UART, USB connector
</commit_message>
<xml_diff>
--- a/demoboard_v2/0714spreadsheet.xlsx
+++ b/demoboard_v2/0714spreadsheet.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="173">
   <si>
     <t>TMS570LS0714</t>
   </si>
@@ -549,6 +549,9 @@
   </si>
   <si>
     <t>GIOB2 test point</t>
+  </si>
+  <si>
+    <t>WATCHDOG</t>
   </si>
 </sst>
 </file>
@@ -894,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1780,6 +1783,9 @@
       </c>
       <c r="E52" t="s">
         <v>71</v>
+      </c>
+      <c r="F52" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updating to recent changes
</commit_message>
<xml_diff>
--- a/demoboard_v2/0714spreadsheet.xlsx
+++ b/demoboard_v2/0714spreadsheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7340" yWindow="460" windowWidth="18260" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pins and KiCad" sheetId="2" r:id="rId1"/>
@@ -898,13 +898,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q147"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -3174,7 +3174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1048490" workbookViewId="0">
+    <sheetView topLeftCell="A1048490" workbookViewId="0">
       <selection activeCell="D1048576" sqref="D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>